<commit_message>
Publish Organism search works
in publish.jsp
</commit_message>
<xml_diff>
--- a/Doc/Logboeken/Logbook_Tom.xlsx
+++ b/Doc/Logboeken/Logbook_Tom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t xml:space="preserve">Meeting </t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>zoeken naar icon methodes</t>
+  </si>
+  <si>
+    <t>validatie txt field samen met Eric</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,7 +1204,9 @@
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>

</xml_diff>

<commit_message>
log ook zoals Eric
</commit_message>
<xml_diff>
--- a/Doc/Logboeken/Logbook_Tom.xlsx
+++ b/Doc/Logboeken/Logbook_Tom.xlsx
@@ -128,9 +128,6 @@
     <t>Tijd in uur</t>
   </si>
   <si>
-    <t xml:space="preserve">Onderwerpen: </t>
-  </si>
-  <si>
     <t>Datum</t>
   </si>
   <si>
@@ -212,7 +209,10 @@
     <t>food van organism</t>
   </si>
   <si>
-    <t>many to many dropdownlsiten food vullen samen lenny, Eric Bert</t>
+    <t>Onderwerpen</t>
+  </si>
+  <si>
+    <t>many to many dropdownlsiten food vullen samen lenny, Eric, Bert</t>
   </si>
 </sst>
 </file>
@@ -379,16 +379,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3352800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1205737</xdr:colOff>
+      <xdr:colOff>6273037</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>719390</xdr:rowOff>
+      <xdr:rowOff>810830</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -405,7 +405,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="5067300" y="91440"/>
           <a:ext cx="2920237" cy="719390"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -417,16 +417,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1325880</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6141720</xdr:colOff>
+      <xdr:colOff>3169920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1623061</xdr:rowOff>
+      <xdr:rowOff>1661161</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -437,7 +437,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3040380" y="1"/>
+          <a:off x="68580" y="38101"/>
           <a:ext cx="4815840" cy="1623060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,13 +963,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1015,7 +1015,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1033,7 +1033,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1129,7 +1129,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1325,7 +1325,7 @@
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1343,7 +1343,7 @@
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1354,42 +1354,42 @@
         <v>10</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1400,35 +1400,35 @@
         <v>10</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1439,28 +1439,28 @@
         <v>10</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1471,7 +1471,7 @@
         <v>4</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1482,14 +1482,14 @@
         <v>9</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1500,28 +1500,28 @@
         <v>6</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1532,35 +1532,35 @@
         <v>8</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1571,14 +1571,14 @@
         <v>9</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UX in dashboard knop naar modal
deze regel aan t ein van dashboard geeft een fout, ik vind het echter
niet
$(document).ready(function(){$(".chosen-select").chosen({width:"100%"}),loadOrganisms(),loadWorlds(),loadSeasons(),loadFamilies(),loadSubFamilies(),loadHabitats(),loadGeolocations(),loadEaten()});
</commit_message>
<xml_diff>
--- a/Doc/Logboeken/Logbook_Tom.xlsx
+++ b/Doc/Logboeken/Logbook_Tom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
   <si>
     <t xml:space="preserve">Meeting </t>
   </si>
@@ -291,6 +291,15 @@
   </si>
   <si>
     <t>griekse texten terug zetten voor opdrachtgever na fix van Lenny en Eric</t>
+  </si>
+  <si>
+    <t>zoeken voor oplossingen bugs</t>
+  </si>
+  <si>
+    <t>subscriber toevoegen</t>
+  </si>
+  <si>
+    <t>UX breed in organism</t>
   </si>
 </sst>
 </file>
@@ -1021,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,19 +1926,67 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="2"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="4"/>
+      <c r="A109" s="2">
+        <v>42086</v>
+      </c>
+      <c r="B109" s="3">
+        <v>4</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
-      <c r="C110" s="4"/>
+      <c r="C110" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="3"/>
-      <c r="B111" s="3"/>
-      <c r="C111" s="4"/>
+      <c r="A111" s="2">
+        <v>42088</v>
+      </c>
+      <c r="B111" s="3">
+        <v>4</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>42089</v>
+      </c>
+      <c r="B112" s="3"/>
+      <c r="C112" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="2"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="4"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="2"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="2"/>
+      <c r="B115" s="3"/>
+      <c r="C115" s="4"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="2"/>
+      <c r="B116" s="3"/>
+      <c r="C116" s="4"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="3"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Mockup & Use case Publish
</commit_message>
<xml_diff>
--- a/Doc/Logboeken/Logbook_Tom.xlsx
+++ b/Doc/Logboeken/Logbook_Tom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
   <si>
     <t xml:space="preserve">Meeting </t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>kleine veranderingen aan downloads naar opdrachtgever wens</t>
+  </si>
+  <si>
+    <t>Documentatie</t>
   </si>
 </sst>
 </file>
@@ -1063,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2106,14 +2109,35 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="2"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="4"/>
+      <c r="A125" s="2">
+        <v>42131</v>
+      </c>
+      <c r="B125" s="3">
+        <v>2</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="3"/>
+      <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="4"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="2"/>
+      <c r="B127" s="3"/>
+      <c r="C127" s="4"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="2"/>
+      <c r="B128" s="3"/>
+      <c r="C128" s="4"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>